<commit_message>
Removal of obsolete scripts, part 2
</commit_message>
<xml_diff>
--- a/fan_database/sanyo denki_flow.xlsx
+++ b/fan_database/sanyo denki_flow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoãoGonçaloCouto\PycharmProjects\fan_selector\fan_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391C780C-4FC5-4538-8C04-D901019590AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4CC025-DC5F-4864-83B7-7162FFBC97F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="-110" windowWidth="36410" windowHeight="21820" firstSheet="61" activeTab="70" xr2:uid="{0FA03CE7-5C65-42AB-9403-FE6892383D75}"/>
+    <workbookView xWindow="1950" yWindow="-110" windowWidth="36560" windowHeight="21820" firstSheet="63" activeTab="72" xr2:uid="{0FA03CE7-5C65-42AB-9403-FE6892383D75}"/>
   </bookViews>
   <sheets>
     <sheet name="9HV1248P1G001" sheetId="1" r:id="rId1"/>
@@ -84,6 +84,8 @@
     <sheet name="9GA0624P1J03" sheetId="88" r:id="rId69"/>
     <sheet name="9GV0624P1G03" sheetId="89" r:id="rId70"/>
     <sheet name="9WV1224P1J601" sheetId="90" r:id="rId71"/>
+    <sheet name="9GT1224P1S001" sheetId="91" r:id="rId72"/>
+    <sheet name="9GT0924P1M001" sheetId="92" r:id="rId73"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="45" hidden="1">'9GA1224P4G001'!$A$1:$C$1</definedName>
@@ -108,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3251" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3396" uniqueCount="77">
   <si>
     <t>Model</t>
   </si>
@@ -333,6 +335,12 @@
   </si>
   <si>
     <t>9WV1224P1J601</t>
+  </si>
+  <si>
+    <t>9GT1224P1S001</t>
+  </si>
+  <si>
+    <t>9GT0924P1M001</t>
   </si>
 </sst>
 </file>
@@ -42387,8 +42395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24401535-6597-4329-BB81-300B44F5B838}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -43315,6 +43323,1987 @@
       </c>
       <c r="D66">
         <v>82.164000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8706098-E8F1-46FF-A370-758301547D64}">
+  <dimension ref="A1:D63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>269.327</v>
+      </c>
+      <c r="D2">
+        <v>1.8780000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>254.18299999999999</v>
+      </c>
+      <c r="D3">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>246.61</v>
+      </c>
+      <c r="D4">
+        <v>34.421999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>231.46600000000001</v>
+      </c>
+      <c r="D5">
+        <v>55.637999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>218.37899999999999</v>
+      </c>
+      <c r="D6">
+        <v>70.943999999999988</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>201.39500000000001</v>
+      </c>
+      <c r="D7">
+        <v>100.69799999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>186.03</v>
+      </c>
+      <c r="D8">
+        <v>122.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>170.88499999999999</v>
+      </c>
+      <c r="D9">
+        <v>143.352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>158.76</v>
+      </c>
+      <c r="D10">
+        <v>170.226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>157.23500000000001</v>
+      </c>
+      <c r="D11">
+        <v>182.952</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>157.18600000000001</v>
+      </c>
+      <c r="D12">
+        <v>196.96799999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>153.41900000000001</v>
+      </c>
+      <c r="D13">
+        <v>216.88799999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>145.9</v>
+      </c>
+      <c r="D14">
+        <v>229.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>136.00200000000001</v>
+      </c>
+      <c r="D15">
+        <v>242.352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>136.00200000000001</v>
+      </c>
+      <c r="D16">
+        <v>242.352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>119.35</v>
+      </c>
+      <c r="D17">
+        <v>259.33800000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <v>119.35</v>
+      </c>
+      <c r="D18">
+        <v>259.33800000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>106.848</v>
+      </c>
+      <c r="D19">
+        <v>271.35599999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>95.13</v>
+      </c>
+      <c r="D20">
+        <v>281.976</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>77.724999999999994</v>
+      </c>
+      <c r="D21">
+        <v>296.13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <v>63.149000000000001</v>
+      </c>
+      <c r="D22">
+        <v>308.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>43.67</v>
+      </c>
+      <c r="D23">
+        <v>324.43799999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <v>26.263999999999999</v>
+      </c>
+      <c r="D24">
+        <v>338.59199999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>8.859</v>
+      </c>
+      <c r="D25">
+        <v>352.74600000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="D26">
+        <v>359.81400000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+      <c r="C27">
+        <v>159.84700000000001</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>146.059</v>
+      </c>
+      <c r="D28">
+        <v>20.358000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29">
+        <v>60</v>
+      </c>
+      <c r="C29">
+        <v>131.66900000000001</v>
+      </c>
+      <c r="D29">
+        <v>42.996000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30">
+        <v>60</v>
+      </c>
+      <c r="C30">
+        <v>123.349</v>
+      </c>
+      <c r="D30">
+        <v>56.94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31">
+        <v>60</v>
+      </c>
+      <c r="C31">
+        <v>111.538</v>
+      </c>
+      <c r="D31">
+        <v>77.88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>100.92100000000001</v>
+      </c>
+      <c r="D32">
+        <v>95.927999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>87.733000000000004</v>
+      </c>
+      <c r="D33">
+        <v>122.208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34">
+        <v>60</v>
+      </c>
+      <c r="C34">
+        <v>85.998000000000005</v>
+      </c>
+      <c r="D34">
+        <v>132.90600000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35">
+        <v>60</v>
+      </c>
+      <c r="C35">
+        <v>85.629000000000005</v>
+      </c>
+      <c r="D35">
+        <v>144.036</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36">
+        <v>60</v>
+      </c>
+      <c r="C36">
+        <v>86.1</v>
+      </c>
+      <c r="D36">
+        <v>150.048</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>86.186000000000007</v>
+      </c>
+      <c r="D37">
+        <v>156.14399999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38">
+        <v>60</v>
+      </c>
+      <c r="C38">
+        <v>83.224999999999994</v>
+      </c>
+      <c r="D38">
+        <v>166.30799999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39">
+        <v>60</v>
+      </c>
+      <c r="C39">
+        <v>77.855999999999995</v>
+      </c>
+      <c r="D39">
+        <v>175.88400000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40">
+        <v>60</v>
+      </c>
+      <c r="C40">
+        <v>68.081999999999994</v>
+      </c>
+      <c r="D40">
+        <v>185.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41">
+        <v>60</v>
+      </c>
+      <c r="C41">
+        <v>58.540999999999997</v>
+      </c>
+      <c r="D41">
+        <v>199.28400000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42">
+        <v>60</v>
+      </c>
+      <c r="C42">
+        <v>45.295000000000002</v>
+      </c>
+      <c r="D42">
+        <v>214.15199999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43">
+        <v>60</v>
+      </c>
+      <c r="C43">
+        <v>28.640999999999998</v>
+      </c>
+      <c r="D43">
+        <v>232.542</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44">
+        <v>60</v>
+      </c>
+      <c r="C44">
+        <v>18.247</v>
+      </c>
+      <c r="D44">
+        <v>242.29199999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45">
+        <v>60</v>
+      </c>
+      <c r="C45">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="D45">
+        <v>259.452</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46">
+        <v>35</v>
+      </c>
+      <c r="C46">
+        <v>84.831000000000003</v>
+      </c>
+      <c r="D46">
+        <v>2.0279999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>76.710999999999999</v>
+      </c>
+      <c r="D47">
+        <v>14.891999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48">
+        <v>35</v>
+      </c>
+      <c r="C48">
+        <v>71.195999999999998</v>
+      </c>
+      <c r="D48">
+        <v>26.076000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49">
+        <v>35</v>
+      </c>
+      <c r="C49">
+        <v>63.829000000000001</v>
+      </c>
+      <c r="D49">
+        <v>36.054000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50">
+        <v>35</v>
+      </c>
+      <c r="C50">
+        <v>58.316000000000003</v>
+      </c>
+      <c r="D50">
+        <v>51.54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51">
+        <v>35</v>
+      </c>
+      <c r="C51">
+        <v>46.192</v>
+      </c>
+      <c r="D51">
+        <v>76.998000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52">
+        <v>35</v>
+      </c>
+      <c r="C52">
+        <v>43.654000000000003</v>
+      </c>
+      <c r="D52">
+        <v>84.168000000000006</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53">
+        <v>35</v>
+      </c>
+      <c r="C53">
+        <v>43.646000000000001</v>
+      </c>
+      <c r="D53">
+        <v>92.412000000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54">
+        <v>35</v>
+      </c>
+      <c r="C54">
+        <v>45.061999999999998</v>
+      </c>
+      <c r="D54">
+        <v>105.324</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55">
+        <v>35</v>
+      </c>
+      <c r="C55">
+        <v>44.646000000000001</v>
+      </c>
+      <c r="D55">
+        <v>109.518</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56">
+        <v>35</v>
+      </c>
+      <c r="C56">
+        <v>39.340000000000003</v>
+      </c>
+      <c r="D56">
+        <v>122.25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57">
+        <v>35</v>
+      </c>
+      <c r="C57">
+        <v>38.255000000000003</v>
+      </c>
+      <c r="D57">
+        <v>123.36599999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58">
+        <v>35</v>
+      </c>
+      <c r="C58">
+        <v>33.481999999999999</v>
+      </c>
+      <c r="D58">
+        <v>133.392</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59">
+        <v>35</v>
+      </c>
+      <c r="C59">
+        <v>25.704999999999998</v>
+      </c>
+      <c r="D59">
+        <v>146.298</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60">
+        <v>35</v>
+      </c>
+      <c r="C60">
+        <v>21.161000000000001</v>
+      </c>
+      <c r="D60">
+        <v>153.37200000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61">
+        <v>35</v>
+      </c>
+      <c r="C61">
+        <v>14.519</v>
+      </c>
+      <c r="D61">
+        <v>161.68799999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62">
+        <v>35</v>
+      </c>
+      <c r="C62">
+        <v>6.0170000000000003</v>
+      </c>
+      <c r="D62">
+        <v>174.59399999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63">
+        <v>35</v>
+      </c>
+      <c r="C63">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="D63">
+        <v>180.40199999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE693ED0-85E8-47F4-A106-96A4902BB0F5}">
+  <dimension ref="A1:D76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>315.12700000000001</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>303.17200000000003</v>
+      </c>
+      <c r="D3">
+        <v>5.5439999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>293.74599999999998</v>
+      </c>
+      <c r="D4">
+        <v>10.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>274.43299999999999</v>
+      </c>
+      <c r="D5">
+        <v>20.957999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>257.87799999999999</v>
+      </c>
+      <c r="D6">
+        <v>33.438000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>252.35900000000001</v>
+      </c>
+      <c r="D7">
+        <v>39.311999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>245.23</v>
+      </c>
+      <c r="D8">
+        <v>45.366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>236.72200000000001</v>
+      </c>
+      <c r="D9">
+        <v>52.524000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>226.60499999999999</v>
+      </c>
+      <c r="D10">
+        <v>61.332000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>210.96799999999999</v>
+      </c>
+      <c r="D11">
+        <v>74.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>196.25399999999999</v>
+      </c>
+      <c r="D12">
+        <v>83.358000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>193.548</v>
+      </c>
+      <c r="D13">
+        <v>85.926000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>187.161</v>
+      </c>
+      <c r="D14">
+        <v>90.588000000000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>185.21299999999999</v>
+      </c>
+      <c r="D15">
+        <v>98.772000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>186.24100000000001</v>
+      </c>
+      <c r="D16">
+        <v>105.012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>188.61</v>
+      </c>
+      <c r="D17">
+        <v>111.71400000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <v>186.124</v>
+      </c>
+      <c r="D18">
+        <v>116.39399999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>184.411</v>
+      </c>
+      <c r="D19">
+        <v>118.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>180.60499999999999</v>
+      </c>
+      <c r="D20">
+        <v>121.53599999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>172.001</v>
+      </c>
+      <c r="D21">
+        <v>126.276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <v>162.21199999999999</v>
+      </c>
+      <c r="D22">
+        <v>131.81399999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>141.98099999999999</v>
+      </c>
+      <c r="D23">
+        <v>142.08600000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <v>122.669</v>
+      </c>
+      <c r="D24">
+        <v>150.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>109.45</v>
+      </c>
+      <c r="D25">
+        <v>155.76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>94.162000000000006</v>
+      </c>
+      <c r="D26">
+        <v>161.91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27">
+        <v>73.930999999999997</v>
+      </c>
+      <c r="D27">
+        <v>169.98000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="C28">
+        <v>53.7</v>
+      </c>
+      <c r="D28">
+        <v>178.78800000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29">
+        <v>100</v>
+      </c>
+      <c r="C29">
+        <v>48.182000000000002</v>
+      </c>
+      <c r="D29">
+        <v>180.99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30">
+        <v>100</v>
+      </c>
+      <c r="C30">
+        <v>37.491999999999997</v>
+      </c>
+      <c r="D30">
+        <v>184.84800000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31">
+        <v>27.951000000000001</v>
+      </c>
+      <c r="D31">
+        <v>189.066</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32">
+        <v>100</v>
+      </c>
+      <c r="C32">
+        <v>15.654999999999999</v>
+      </c>
+      <c r="D32">
+        <v>193.44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="D33">
+        <v>197.892</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34">
+        <v>60</v>
+      </c>
+      <c r="C34">
+        <v>183.42099999999999</v>
+      </c>
+      <c r="D34">
+        <v>1.1220000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35">
+        <v>60</v>
+      </c>
+      <c r="C35">
+        <v>176.29400000000001</v>
+      </c>
+      <c r="D35">
+        <v>5.3460000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36">
+        <v>60</v>
+      </c>
+      <c r="C36">
+        <v>165.947</v>
+      </c>
+      <c r="D36">
+        <v>12.87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>156.75</v>
+      </c>
+      <c r="D37">
+        <v>19.475999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38">
+        <v>60</v>
+      </c>
+      <c r="C38">
+        <v>150.31100000000001</v>
+      </c>
+      <c r="D38">
+        <v>26.081999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39">
+        <v>60</v>
+      </c>
+      <c r="C39">
+        <v>145.71100000000001</v>
+      </c>
+      <c r="D39">
+        <v>31.955999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40">
+        <v>60</v>
+      </c>
+      <c r="C40">
+        <v>136.51300000000001</v>
+      </c>
+      <c r="D40">
+        <v>40.764000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41">
+        <v>60</v>
+      </c>
+      <c r="C41">
+        <v>131.91300000000001</v>
+      </c>
+      <c r="D41">
+        <v>47.003999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42">
+        <v>60</v>
+      </c>
+      <c r="C42">
+        <v>125.934</v>
+      </c>
+      <c r="D42">
+        <v>52.698</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43">
+        <v>60</v>
+      </c>
+      <c r="C43">
+        <v>119.496</v>
+      </c>
+      <c r="D43">
+        <v>57.101999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44">
+        <v>60</v>
+      </c>
+      <c r="C44">
+        <v>115.35599999999999</v>
+      </c>
+      <c r="D44">
+        <v>61.32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45">
+        <v>60</v>
+      </c>
+      <c r="C45">
+        <v>107.768</v>
+      </c>
+      <c r="D45">
+        <v>67.745999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46">
+        <v>60</v>
+      </c>
+      <c r="C46">
+        <v>106.386</v>
+      </c>
+      <c r="D46">
+        <v>73.62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47">
+        <v>60</v>
+      </c>
+      <c r="C47">
+        <v>106.155</v>
+      </c>
+      <c r="D47">
+        <v>77.471999999999994</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48">
+        <v>60</v>
+      </c>
+      <c r="C48">
+        <v>107.301</v>
+      </c>
+      <c r="D48">
+        <v>83.346000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49">
+        <v>60</v>
+      </c>
+      <c r="C49">
+        <v>107.298</v>
+      </c>
+      <c r="D49">
+        <v>88.854000000000013</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50">
+        <v>60</v>
+      </c>
+      <c r="C50">
+        <v>98.102000000000004</v>
+      </c>
+      <c r="D50">
+        <v>94.542000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51">
+        <v>60</v>
+      </c>
+      <c r="C51">
+        <v>95.111999999999995</v>
+      </c>
+      <c r="D51">
+        <v>98.027999999999992</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52">
+        <v>60</v>
+      </c>
+      <c r="C52">
+        <v>86.834999999999994</v>
+      </c>
+      <c r="D52">
+        <v>103.35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53">
+        <v>60</v>
+      </c>
+      <c r="C53">
+        <v>77.637</v>
+      </c>
+      <c r="D53">
+        <v>110.50800000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54">
+        <v>60</v>
+      </c>
+      <c r="C54">
+        <v>68.900999999999996</v>
+      </c>
+      <c r="D54">
+        <v>114.732</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55">
+        <v>60</v>
+      </c>
+      <c r="C55">
+        <v>58.323999999999998</v>
+      </c>
+      <c r="D55">
+        <v>121.52399999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>39.012</v>
+      </c>
+      <c r="D56">
+        <v>131.06400000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>20.619</v>
+      </c>
+      <c r="D57">
+        <v>142.07400000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58">
+        <v>60</v>
+      </c>
+      <c r="C58">
+        <v>13.491</v>
+      </c>
+      <c r="D58">
+        <v>145.74600000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>1.3069999999999999</v>
+      </c>
+      <c r="D59">
+        <v>150.88200000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60">
+        <v>30</v>
+      </c>
+      <c r="C60">
+        <v>71.254000000000005</v>
+      </c>
+      <c r="D60">
+        <v>1.1099999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61">
+        <v>30</v>
+      </c>
+      <c r="C61">
+        <v>71.254000000000005</v>
+      </c>
+      <c r="D61">
+        <v>1.1099999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62">
+        <v>30</v>
+      </c>
+      <c r="C62">
+        <v>65.504000000000005</v>
+      </c>
+      <c r="D62">
+        <v>6.984</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63">
+        <v>30</v>
+      </c>
+      <c r="C63">
+        <v>59.293999999999997</v>
+      </c>
+      <c r="D63">
+        <v>16.523999999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64">
+        <v>30</v>
+      </c>
+      <c r="C64">
+        <v>59.293999999999997</v>
+      </c>
+      <c r="D64">
+        <v>16.523999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65">
+        <v>30</v>
+      </c>
+      <c r="C65">
+        <v>53.314</v>
+      </c>
+      <c r="D65">
+        <v>24.053999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66">
+        <v>30</v>
+      </c>
+      <c r="C66">
+        <v>48.253</v>
+      </c>
+      <c r="D66">
+        <v>32.676000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67">
+        <v>30</v>
+      </c>
+      <c r="C67">
+        <v>48.253</v>
+      </c>
+      <c r="D67">
+        <v>32.676000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68">
+        <v>30</v>
+      </c>
+      <c r="C68">
+        <v>38.826000000000001</v>
+      </c>
+      <c r="D68">
+        <v>39.101999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69">
+        <v>30</v>
+      </c>
+      <c r="C69">
+        <v>38.823</v>
+      </c>
+      <c r="D69">
+        <v>45.161999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70">
+        <v>30</v>
+      </c>
+      <c r="C70">
+        <v>40.43</v>
+      </c>
+      <c r="D70">
+        <v>49.565999999999995</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71">
+        <v>30</v>
+      </c>
+      <c r="C71">
+        <v>37.899000000000001</v>
+      </c>
+      <c r="D71">
+        <v>55.992000000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72">
+        <v>30</v>
+      </c>
+      <c r="C72">
+        <v>34.448</v>
+      </c>
+      <c r="D72">
+        <v>61.314</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73">
+        <v>30</v>
+      </c>
+      <c r="C73">
+        <v>26.17</v>
+      </c>
+      <c r="D73">
+        <v>68.471999999999994</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74">
+        <v>30</v>
+      </c>
+      <c r="C74">
+        <v>18.812000000000001</v>
+      </c>
+      <c r="D74">
+        <v>75.257999999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75">
+        <v>30</v>
+      </c>
+      <c r="C75">
+        <v>11.454000000000001</v>
+      </c>
+      <c r="D75">
+        <v>80.951999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76">
+        <v>30</v>
+      </c>
+      <c r="C76">
+        <v>0.187</v>
+      </c>
+      <c r="D76">
+        <v>89.022000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>